<commit_message>
update input params 2020
in progress
</commit_message>
<xml_diff>
--- a/simfin/params/historical_accounts.xlsx
+++ b/simfin/params/historical_accounts.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10314"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juliennavaux/Documents/SimFin/Model/simfin/params/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wilet\Dropbox\simfin\Model\simfin\params\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15AC820F-22FD-BA4F-9C7C-7C087B3BE819}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68062DFD-1B1D-4D30-A934-D421277BFF62}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5660" yWindow="760" windowWidth="40300" windowHeight="21180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Inputs" sheetId="2" r:id="rId1"/>
@@ -289,12 +289,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -310,7 +316,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -341,6 +347,8 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" indent="4"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -359,14 +367,10 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
-    <a:clrScheme name="Bureau">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -404,7 +408,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Bureau">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -510,7 +514,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Bureau">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -662,14 +666,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:P43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="O31" sqref="O31"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="38.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -719,7 +725,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -765,11 +771,11 @@
       <c r="O2">
         <v>27206</v>
       </c>
-      <c r="P2" s="4">
-        <v>28581.692073361392</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="P2">
+        <v>28841</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>23</v>
       </c>
@@ -815,11 +821,11 @@
       <c r="O3">
         <v>4567</v>
       </c>
-      <c r="P3" s="4">
-        <v>4797.9338270617318</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="P3">
+        <v>4973</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>24</v>
       </c>
@@ -865,11 +871,11 @@
       <c r="O4">
         <v>7457</v>
       </c>
-      <c r="P4" s="4">
-        <v>7048.6858690300978</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="P4">
+        <v>6605</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -915,11 +921,11 @@
       <c r="O5">
         <v>1726</v>
       </c>
-      <c r="P5" s="4">
-        <v>1631.4914590245337</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="P5">
+        <v>2002</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -965,11 +971,11 @@
       <c r="O6">
         <v>6359</v>
       </c>
-      <c r="P6" s="4">
-        <v>6568.9174843737592</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="P6">
+        <v>6522</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -1015,11 +1021,11 @@
       <c r="O7">
         <v>1853</v>
       </c>
-      <c r="P7" s="4">
-        <v>1550.3163363697208</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="P7">
+        <v>1539</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -1065,11 +1071,11 @@
       <c r="O8">
         <v>21001</v>
       </c>
-      <c r="P8" s="4">
-        <v>22037.208693975248</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="P8">
+        <v>21348</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -1115,11 +1121,11 @@
       <c r="O9">
         <v>4361</v>
       </c>
-      <c r="P9" s="4">
-        <v>4495.5188365682388</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="P9">
+        <v>4535</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -1165,11 +1171,11 @@
       <c r="O10">
         <v>5548</v>
       </c>
-      <c r="P10" s="4">
-        <v>4555</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="P10">
+        <v>4419</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>40</v>
       </c>
@@ -1215,11 +1221,11 @@
       <c r="O11">
         <v>11548</v>
       </c>
-      <c r="P11" s="4">
-        <v>11119.235420235274</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="P11">
+        <v>10962</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>6</v>
       </c>
@@ -1265,11 +1271,11 @@
       <c r="O12">
         <v>11732</v>
       </c>
-      <c r="P12" s="4">
-        <v>13155.898792684386</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="P12">
+        <v>13124</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>7</v>
       </c>
@@ -1315,11 +1321,11 @@
       <c r="O13">
         <v>6306</v>
       </c>
-      <c r="P13" s="4">
-        <v>6478.7087699725071</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="P13">
+        <v>6617</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>8</v>
       </c>
@@ -1365,11 +1371,11 @@
       <c r="O14">
         <v>5082</v>
       </c>
-      <c r="P14" s="4">
-        <v>5523.3924373431091</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="P14">
+        <v>5487</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>9</v>
       </c>
@@ -1415,11 +1421,11 @@
       <c r="O15">
         <v>41522</v>
       </c>
-      <c r="P15" s="4">
-        <v>43652.254206381862</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="P15">
+        <v>43699</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>10</v>
       </c>
@@ -1465,11 +1471,11 @@
       <c r="O16">
         <v>23887</v>
       </c>
-      <c r="P16" s="4">
-        <v>25208.822479140319</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="P16">
+        <v>25267</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>11</v>
       </c>
@@ -1515,11 +1521,11 @@
       <c r="O17">
         <v>14730</v>
       </c>
-      <c r="P17" s="4">
-        <v>15981.784347802952</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="P17">
+        <v>17293</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>12</v>
       </c>
@@ -1565,11 +1571,11 @@
       <c r="O18">
         <v>10095</v>
       </c>
-      <c r="P18" s="4">
-        <v>10782.421591255705</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="P18">
+        <v>10926</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>13</v>
       </c>
@@ -1615,11 +1621,11 @@
       <c r="O19">
         <v>7510</v>
       </c>
-      <c r="P19" s="4">
-        <v>8098.7173754191663</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="P19">
+        <v>9503</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>14</v>
       </c>
@@ -1665,11 +1671,11 @@
       <c r="O20">
         <v>8722</v>
       </c>
-      <c r="P20" s="4">
-        <v>7648</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="P20">
+        <v>7676</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>26</v>
       </c>
@@ -1719,7 +1725,7 @@
         <v>8293</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>27</v>
       </c>
@@ -1766,10 +1772,10 @@
         <v>2083</v>
       </c>
       <c r="P22">
-        <v>2151.7067983289021</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
+        <v>2142</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>28</v>
       </c>
@@ -1816,10 +1822,10 @@
         <v>1394</v>
       </c>
       <c r="P23">
-        <v>454.29320167109762</v>
-      </c>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>29</v>
       </c>
@@ -1869,7 +1875,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>30</v>
       </c>
@@ -1919,7 +1925,7 @@
         <v>8899</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>37</v>
       </c>
@@ -1965,11 +1971,11 @@
       <c r="O26">
         <v>7174</v>
       </c>
-      <c r="P26" s="4">
+      <c r="P26">
         <v>11977</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>31</v>
       </c>
@@ -2019,7 +2025,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>15</v>
       </c>
@@ -2065,11 +2071,11 @@
       <c r="O28">
         <v>4803</v>
       </c>
-      <c r="P28" s="4">
-        <v>2963</v>
-      </c>
-    </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="P28">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>32</v>
       </c>
@@ -2116,10 +2122,10 @@
         <v>4803</v>
       </c>
       <c r="P29">
-        <v>2963</v>
-      </c>
-    </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>33</v>
       </c>
@@ -2165,11 +2171,11 @@
       <c r="O30">
         <v>11977</v>
       </c>
-      <c r="P30" s="4">
-        <v>14940</v>
-      </c>
-    </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="P30">
+        <v>11981</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>34</v>
       </c>
@@ -2216,7 +2222,7 @@
         <v>189029</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>35</v>
       </c>
@@ -2266,7 +2272,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>36</v>
       </c>
@@ -2312,11 +2318,11 @@
       <c r="O33">
         <v>189029</v>
       </c>
-      <c r="P33" s="4">
-        <v>193229</v>
-      </c>
-    </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="P33">
+        <v>192975</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>16</v>
       </c>
@@ -2363,10 +2369,10 @@
         <v>6159</v>
       </c>
       <c r="P34">
-        <v>6422.757080654952</v>
-      </c>
-    </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.2">
+        <v>7988</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>17</v>
       </c>
@@ -2412,11 +2418,11 @@
       <c r="O35">
         <v>199098</v>
       </c>
-      <c r="P35" s="4">
-        <v>198916</v>
-      </c>
-    </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="P35">
+        <v>198792</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>38</v>
       </c>
@@ -2462,11 +2468,11 @@
       <c r="O36" s="4">
         <v>439509.93377483444</v>
       </c>
-      <c r="P36" s="4">
-        <v>458331.79723502306</v>
-      </c>
-    </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="P36" s="18">
+        <v>458046.08294930874</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>39</v>
       </c>
@@ -2513,10 +2519,10 @@
         <v>3.1977506173939678E-2</v>
       </c>
       <c r="P37">
-        <v>2.2377117601684784E-2</v>
-      </c>
-    </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.2">
+        <v>3.3542115050475822E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>42</v>
       </c>
@@ -2552,11 +2558,11 @@
       <c r="O38" s="3">
         <v>18362</v>
       </c>
-      <c r="P38" s="3">
+      <c r="P38">
         <v>13905.776600000012</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A39" s="5" t="s">
         <v>43</v>
       </c>
@@ -2602,11 +2608,11 @@
       <c r="O39" s="4">
         <v>1291</v>
       </c>
-      <c r="P39" s="3">
+      <c r="P39">
         <v>901</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>46</v>
       </c>
@@ -2653,10 +2659,10 @@
         <v>71316</v>
       </c>
       <c r="P40">
-        <v>74450</v>
-      </c>
-    </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.2">
+        <v>75053</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>47</v>
       </c>
@@ -2702,11 +2708,11 @@
       <c r="O41">
         <v>27334</v>
       </c>
-      <c r="P41">
-        <v>29547</v>
-      </c>
-    </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="P41" s="19">
+        <v>28533</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>48</v>
       </c>
@@ -2750,10 +2756,10 @@
         <v>3002</v>
       </c>
       <c r="P42">
-        <v>3134</v>
-      </c>
-    </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.2">
+        <v>3737</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>49</v>
       </c>
@@ -2797,7 +2803,7 @@
         <v>2047</v>
       </c>
       <c r="P43">
-        <v>2213</v>
+        <v>1199</v>
       </c>
     </row>
   </sheetData>
@@ -2816,13 +2822,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="12.83203125" customWidth="1"/>
     <col min="3" max="3" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>18</v>
       </c>
@@ -2833,7 +2839,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>2006</v>
       </c>
@@ -2842,7 +2848,7 @@
       </c>
       <c r="C2" s="2"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2007</v>
       </c>
@@ -2851,7 +2857,7 @@
       </c>
       <c r="C3" s="2"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>2008</v>
       </c>
@@ -2862,7 +2868,7 @@
         <v>6.1643835616438353E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>2009</v>
       </c>
@@ -2873,7 +2879,7 @@
         <v>-4.0551500405515001E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>2010</v>
       </c>
@@ -2884,7 +2890,7 @@
         <v>3.0737704918032786E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>2011</v>
       </c>
@@ -2895,7 +2901,7 @@
         <v>3.5113933507657825E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>2012</v>
       </c>
@@ -2906,7 +2912,7 @@
         <v>4.3351760256037243E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>2013</v>
       </c>
@@ -2917,7 +2923,7 @@
         <v>5.4243628711713815E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>2014</v>
       </c>
@@ -2929,7 +2935,7 @@
       </c>
       <c r="F10" s="2"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>2015</v>
       </c>
@@ -2940,7 +2946,7 @@
         <v>5.5663544795900334E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>2016</v>
       </c>
@@ -2951,7 +2957,7 @@
         <v>4.295185932545402E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>2017</v>
       </c>
@@ -2962,7 +2968,7 @@
         <v>4.9518892278807791E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>2018</v>
       </c>
@@ -2973,7 +2979,7 @@
         <v>3.9152332984890244E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>2019</v>
       </c>
@@ -2984,7 +2990,7 @@
         <v>0.10877028714107366</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>2020</v>
       </c>
@@ -2995,7 +3001,7 @@
         <v>3.5499999999999997E-2</v>
       </c>
     </row>
-    <row r="18" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C18" s="2"/>
     </row>
   </sheetData>
@@ -3014,9 +3020,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>18</v>
       </c>
@@ -3024,7 +3030,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>2017</v>
       </c>
@@ -3032,7 +3038,7 @@
         <v>1579</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2018</v>
       </c>
@@ -3040,7 +3046,7 @@
         <v>1881</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>2019</v>
       </c>
@@ -3048,7 +3054,7 @@
         <v>2083</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>2020</v>
       </c>
@@ -3056,7 +3062,7 @@
         <v>2174</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>2021</v>
       </c>
@@ -3064,7 +3070,7 @@
         <v>2267</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>2022</v>
       </c>
@@ -3072,7 +3078,7 @@
         <v>2437</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>2023</v>
       </c>
@@ -3080,7 +3086,7 @@
         <v>2614</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>2024</v>
       </c>
@@ -3088,7 +3094,7 @@
         <v>2775</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>2025</v>
       </c>
@@ -3112,12 +3118,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="37.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>59</v>
       </c>
@@ -3167,7 +3173,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>50</v>
       </c>
@@ -3202,7 +3208,7 @@
         <v>110835</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>51</v>
       </c>
@@ -3237,7 +3243,7 @@
         <v>2644.0913</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>52</v>
       </c>
@@ -3272,7 +3278,7 @@
         <v>7038.0225</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>54</v>
       </c>
@@ -3307,7 +3313,7 @@
         <v>7165.1682000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>53</v>
       </c>
@@ -3342,7 +3348,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>62</v>
       </c>
@@ -3377,7 +3383,7 @@
         <v>113421.94560000001</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>55</v>
       </c>
@@ -3412,7 +3418,7 @@
         <v>-5179</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>58</v>
       </c>
@@ -3447,7 +3453,7 @@
         <v>94104.262499999997</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>56</v>
       </c>
@@ -3482,7 +3488,7 @@
         <v>1564.4084999999998</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>63</v>
       </c>
@@ -3517,7 +3523,7 @@
         <v>1797.3149999999998</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>57</v>
       </c>
@@ -3563,13 +3569,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="78.5" customWidth="1"/>
     <col min="2" max="2" width="32.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>59</v>
       </c>
@@ -3577,7 +3583,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="s">
         <v>51</v>
       </c>
@@ -3590,7 +3596,7 @@
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="12" t="s">
         <v>61</v>
       </c>
@@ -3603,7 +3609,7 @@
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="12" t="s">
         <v>54</v>
       </c>
@@ -3616,7 +3622,7 @@
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="12" t="s">
         <v>53</v>
       </c>
@@ -3629,7 +3635,7 @@
       <c r="F5" s="6"/>
       <c r="G5" s="6"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="12"/>
       <c r="B6" s="4"/>
       <c r="C6" s="6"/>
@@ -3638,7 +3644,7 @@
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="8"/>
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
@@ -3647,7 +3653,7 @@
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="8"/>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
@@ -3656,7 +3662,7 @@
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" s="8"/>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
@@ -3665,7 +3671,7 @@
       <c r="F9" s="6"/>
       <c r="G9" s="6"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" s="8"/>
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
@@ -3674,7 +3680,7 @@
       <c r="F10" s="6"/>
       <c r="G10" s="6"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" s="8"/>
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
@@ -3683,7 +3689,7 @@
       <c r="F11" s="6"/>
       <c r="G11" s="6"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" s="9"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
@@ -3692,7 +3698,7 @@
       <c r="F12" s="6"/>
       <c r="G12" s="6"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" s="10"/>
       <c r="B13" s="7"/>
       <c r="C13" s="6"/>
@@ -3701,7 +3707,7 @@
       <c r="F13" s="6"/>
       <c r="G13" s="6"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" s="10"/>
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
@@ -3710,7 +3716,7 @@
       <c r="F14" s="6"/>
       <c r="G14" s="6"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" s="10"/>
       <c r="B15" s="7"/>
       <c r="C15" s="6"/>
@@ -3719,7 +3725,7 @@
       <c r="F15" s="6"/>
       <c r="G15" s="6"/>
     </row>
-    <row r="16" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A16" s="13"/>
       <c r="B16" s="14"/>
       <c r="C16" s="13"/>
@@ -3728,7 +3734,7 @@
       <c r="F16" s="13"/>
       <c r="G16" s="13"/>
     </row>
-    <row r="17" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A17" s="15"/>
       <c r="B17" s="15"/>
       <c r="C17" s="15"/>
@@ -3737,7 +3743,7 @@
       <c r="F17" s="13"/>
       <c r="G17" s="13"/>
     </row>
-    <row r="18" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A18" s="13"/>
       <c r="B18" s="13"/>
       <c r="C18" s="13"/>
@@ -3746,7 +3752,7 @@
       <c r="F18" s="13"/>
       <c r="G18" s="13"/>
     </row>
-    <row r="19" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A19" s="16"/>
       <c r="B19" s="13"/>
       <c r="C19" s="13"/>
@@ -3755,7 +3761,7 @@
       <c r="F19" s="13"/>
       <c r="G19" s="13"/>
     </row>
-    <row r="20" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A20" s="17"/>
       <c r="B20" s="14"/>
       <c r="C20" s="13"/>
@@ -3764,7 +3770,7 @@
       <c r="F20" s="13"/>
       <c r="G20" s="13"/>
     </row>
-    <row r="21" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A21" s="17"/>
       <c r="B21" s="14"/>
       <c r="C21" s="13"/>
@@ -3773,13 +3779,13 @@
       <c r="F21" s="13"/>
       <c r="G21" s="13"/>
     </row>
-    <row r="22" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="23" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="24" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="25" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="26" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="27" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="28" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="22" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="23" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="24" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="25" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="26" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="27" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="28" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3791,12 +3797,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="21.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>18</v>
       </c>
@@ -3804,7 +3810,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>2006</v>
       </c>
@@ -3812,7 +3818,7 @@
         <v>2831</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2007</v>
       </c>
@@ -3820,7 +3826,7 @@
         <v>2693</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>2008</v>
       </c>
@@ -3828,7 +3834,7 @@
         <v>2486</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>2009</v>
       </c>
@@ -3836,7 +3842,7 @@
         <v>2143</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>2010</v>
       </c>
@@ -3844,7 +3850,7 @@
         <v>2307</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>2011</v>
       </c>
@@ -3852,7 +3858,7 @@
         <v>2652</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>2012</v>
       </c>
@@ -3860,7 +3866,7 @@
         <v>2816</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>2013</v>
       </c>
@@ -3868,7 +3874,7 @@
         <v>3084</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>2014</v>
       </c>
@@ -3876,7 +3882,7 @@
         <v>3379</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>2015</v>
       </c>
@@ -3884,7 +3890,7 @@
         <v>3169</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>2016</v>
       </c>
@@ -3892,7 +3898,7 @@
         <v>2731</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>2017</v>
       </c>
@@ -3900,7 +3906,7 @@
         <v>2309</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>2018</v>
       </c>
@@ -3908,7 +3914,7 @@
         <v>1772</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>2019</v>
       </c>
@@ -3916,7 +3922,7 @@
         <v>1291</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>2020</v>
       </c>
@@ -3924,7 +3930,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>2021</v>
       </c>
@@ -3932,7 +3938,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>2022</v>
       </c>
@@ -3940,7 +3946,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>2023</v>
       </c>
@@ -3948,7 +3954,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>2024</v>
       </c>
@@ -3956,7 +3962,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>2025</v>
       </c>
@@ -3975,13 +3981,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="3" width="18.6640625" customWidth="1"/>
     <col min="4" max="4" width="20.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>18</v>
       </c>
@@ -3995,7 +4001,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>2019</v>
       </c>
@@ -4009,7 +4015,7 @@
         <v>6.8155806925309093E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2020</v>
       </c>
@@ -4023,7 +4029,7 @@
         <v>7.8852288558218415E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>2021</v>
       </c>
@@ -4037,7 +4043,7 @@
         <v>7.6978718363801485E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>2022</v>
       </c>
@@ -4051,7 +4057,7 @@
         <v>9.714309874944432E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>2023</v>
       </c>
@@ -4065,7 +4071,7 @@
         <v>9.252744589238358E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>2024</v>
       </c>
@@ -4079,7 +4085,7 @@
         <v>9.0224926425935426E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>2025</v>
       </c>
@@ -4093,7 +4099,7 @@
         <v>8.9337315566447133E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>2026</v>
       </c>

</xml_diff>